<commit_message>
refresh hour in sales
</commit_message>
<xml_diff>
--- a/IncaArt/IncaArt/Resources/Excel/SalesReport.xlsx
+++ b/IncaArt/IncaArt/Resources/Excel/SalesReport.xlsx
@@ -216,6 +216,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -233,12 +239,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,76 +558,76 @@
   <dimension ref="B1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="1" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="9"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
     </row>
-    <row r="6" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>